<commit_message>
Synchronisation commentaires code avec documentation
</commit_message>
<xml_diff>
--- a/docs/MatriceLabellisationV9.2.xlsx
+++ b/docs/MatriceLabellisationV9.2.xlsx
@@ -22,7 +22,7 @@
     <author>Mathieu</author>
   </authors>
   <commentList>
-    <comment ref="I45" authorId="0">
+    <comment ref="I41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +46,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H53" authorId="0">
+    <comment ref="H50" authorId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A60" authorId="0">
+    <comment ref="A57" authorId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A67" authorId="1">
+    <comment ref="A64" authorId="1">
       <text>
         <r>
           <rPr>
@@ -118,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B67" authorId="1">
+    <comment ref="B64" authorId="1">
       <text>
         <r>
           <rPr>
@@ -142,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C81" authorId="0">
+    <comment ref="C78" authorId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B82" authorId="0">
+    <comment ref="B79" authorId="0">
       <text>
         <r>
           <rPr>
@@ -194,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B87" authorId="0">
+    <comment ref="B84" authorId="0">
       <text>
         <r>
           <rPr>
@@ -218,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C87" authorId="0">
+    <comment ref="C84" authorId="0">
       <text>
         <r>
           <rPr>
@@ -242,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A94" authorId="0">
+    <comment ref="A91" authorId="0">
       <text>
         <r>
           <rPr>
@@ -266,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A95" authorId="0">
+    <comment ref="A92" authorId="0">
       <text>
         <r>
           <rPr>
@@ -290,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B95" authorId="0">
+    <comment ref="B92" authorId="0">
       <text>
         <r>
           <rPr>
@@ -314,7 +314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C95" authorId="0">
+    <comment ref="C92" authorId="0">
       <text>
         <r>
           <rPr>
@@ -338,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B104" authorId="0">
+    <comment ref="B101" authorId="0">
       <text>
         <r>
           <rPr>
@@ -367,7 +367,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="152">
   <si>
     <t>C =&gt; Complet</t>
   </si>
@@ -1004,70 +1004,7 @@
 MC filtré</t>
   </si>
   <si>
-    <t>CAS 1 : Traitement de chaque action de la trace</t>
-  </si>
-  <si>
-    <t>CAS 1.1 : Cas des actions refusées par le jeu</t>
-  </si>
-  <si>
-    <t>=&gt; Traiter cas 1.1 : "Cas des actions refusées par le jeu"</t>
-  </si>
-  <si>
-    <t>CAS 1.2 : Cas des actions acceptées par le jeu</t>
-  </si>
-  <si>
-    <t>=&gt; Générer M'C PUIS Traiter cas 1.2 : "Cas des actions acceptées par le jeu"</t>
-  </si>
-  <si>
-    <t>=&gt; Traiter cas "Historique" et passer en paramètre RdpF</t>
-  </si>
-  <si>
-    <t>=&gt; Traiter cas "Dans espace filtré" et passer en paramètre RdpF</t>
-  </si>
-  <si>
-    <t>=&gt; Traiter cas "Hors espace filtré depuis état initial"</t>
-  </si>
-  <si>
-    <t>(Pour chaque transition de la trace =&gt; Traiter cas 1) PUIS cas "Fin"</t>
-  </si>
-  <si>
-    <t>CAS "Dans espace filtré" (Ce cas peut être appelé avec le graphe d'accessibilité/couverture calculé depuis l'état initial de la simulatipn (MiC) ou à partir de l'état courant de la simulation (MC))</t>
-  </si>
-  <si>
-    <t>=&gt; Traiter cas "Vers solution"</t>
-  </si>
-  <si>
-    <t>=&gt; Traiter cas "Stagnation"</t>
-  </si>
-  <si>
-    <t>=&gt; Traiter cas "Historique" et passer en paramètre RdpX</t>
-  </si>
-  <si>
-    <t>CAS "Vers solution"</t>
-  </si>
-  <si>
-    <t>CAS "Stagnation"</t>
-  </si>
-  <si>
-    <t>CAS "Historique" (Ce cas peut être appelé avec le graphe d'accessibilité/couverture calculé depuis l'état initial de la simulatipn (MiF) ou à partir de l'état courant de la simulation (MC))</t>
-  </si>
-  <si>
-    <t>CAS "Hors espace filtré depuis état initial"</t>
-  </si>
-  <si>
-    <t>CAS "Fin" : gestion des actions manquantes en fin de niveau</t>
-  </si>
-  <si>
     <t>=&gt; Traiter cas 5 "Tendance" et passer en paramètre RdpA</t>
-  </si>
-  <si>
-    <t>CAS "Tendance"</t>
-  </si>
-  <si>
-    <t>=&gt; Traiter cas "Tendance" et passer en paramètre RdpF</t>
-  </si>
-  <si>
-    <t>=&gt; Traiter cas "Tendance" et passer en paramètre RdpW</t>
   </si>
   <si>
     <r>
@@ -1114,6 +1051,66 @@
   </si>
   <si>
     <t>On est dans le cas où la dernière transition de la trace est une action non experte qui place le jeu dans un état hors de l'espace filtré. On remonte donc le parcours du joueur jusqu'à trouver un marquage à partir duquel on peut redescendre jusqu'à la fin du niveau.</t>
+  </si>
+  <si>
+    <t>CAS 2 "Dans espace filtré" (Ce cas peut être appelé avec le graphe d'accessibilité/couverture calculé depuis l'état initial de la simulatipn (MiC) ou à partir de l'état courant de la simulation (MC))</t>
+  </si>
+  <si>
+    <t>CAS 2_1 "Vers solution"</t>
+  </si>
+  <si>
+    <t>CAS 2.2 "Stagnation"</t>
+  </si>
+  <si>
+    <t>CAS 0 : Traitement de chaque action de la trace</t>
+  </si>
+  <si>
+    <t>CAS 6 "Fin" : gestion des actions manquantes en fin de niveau</t>
+  </si>
+  <si>
+    <t>(Pour chaque transition de la trace =&gt; Traiter cas 0) PUIS cas 6</t>
+  </si>
+  <si>
+    <t>=&gt; Générer M'C PUIS Traiter cas 1 : "Cas des actions acceptées par le jeu"</t>
+  </si>
+  <si>
+    <t>CAS 1 : Cas des actions acceptées par le jeu</t>
+  </si>
+  <si>
+    <t>=&gt; Ce cas ne devrait pas arriver (action système non sensibilisée) =&gt; problème dans les traces ?</t>
+  </si>
+  <si>
+    <t>=&gt; Traiter cas 2 "Dans espace filtré" et passer en paramètre RdpF</t>
+  </si>
+  <si>
+    <t>=&gt; Traiter cas 3 "Historique" et passer en paramètre RdpF</t>
+  </si>
+  <si>
+    <t>CAS 3 "Historique" (Ce cas peut être appelé avec le graphe d'accessibilité/couverture calculé depuis l'état initial de la simulatipn (MiF) ou à partir de l'état courant de la simulation (MC))</t>
+  </si>
+  <si>
+    <t>=&gt; Traiter cas 5 "Tendance" et passer en paramètre RdpF</t>
+  </si>
+  <si>
+    <t>CAS 5 "Tendance"</t>
+  </si>
+  <si>
+    <t>=&gt; Traiter cas 4 "Hors espace filtré depuis état initial"</t>
+  </si>
+  <si>
+    <t>CAS 4 "Hors espace filtré depuis état initial"</t>
+  </si>
+  <si>
+    <t>=&gt; Traiter cas 2_1 "Vers solution"</t>
+  </si>
+  <si>
+    <t>=&gt; Traiter cas 2_2 "Stagnation"</t>
+  </si>
+  <si>
+    <t>=&gt; Traiter cas 3 "Historique" et passer en paramètre RdpX</t>
+  </si>
+  <si>
+    <t>=&gt; Traiter cas 5 "Tendance" et passer en paramètre RdpW</t>
   </si>
 </sst>
 </file>
@@ -1272,7 +1269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1336,12 +1333,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="20" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1352,6 +1349,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1446,7 +1444,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1494,7 +1492,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1542,7 +1540,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1590,7 +1588,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1638,7 +1636,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1686,7 +1684,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2614,7 +2612,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>v(fn, M'C)</a:t>
+            <a:t>v(fn, GF, M'C)</a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
@@ -2625,11 +2623,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>976643</xdr:colOff>
+      <xdr:colOff>877835</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>175589</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2417713" cy="272062"/>
+    <xdr:ext cx="2615331" cy="272062"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="33" name="ZoneTexte 32"/>
@@ -2637,8 +2635,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6301118" y="4747589"/>
-          <a:ext cx="2417713" cy="272062"/>
+          <a:off x="6211835" y="4747589"/>
+          <a:ext cx="2615331" cy="272062"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2721,7 +2719,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> GF &amp;&amp; !v(fn, M'C)</a:t>
+            <a:t> GF &amp;&amp; !v(fn, GF, M'C)</a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
@@ -2840,11 +2838,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>403112</xdr:colOff>
+      <xdr:colOff>121564</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>45602</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1755032" cy="436786"/>
+    <xdr:ext cx="2318135" cy="436786"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="47" name="ZoneTexte 46"/>
@@ -2852,8 +2850,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8966087" y="807602"/>
-          <a:ext cx="1755032" cy="436786"/>
+          <a:off x="8682858" y="807602"/>
+          <a:ext cx="2318135" cy="436786"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2883,7 +2881,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>v(fn, MC) &amp;&amp; v(fn, M'C) &amp;&amp;</a:t>
+            <a:t>v(fn, GW, MC) &amp;&amp; v(fn, GW, M'C) &amp;&amp;</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2899,12 +2897,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>257176</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>961745</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1755031" cy="436786"/>
+    <xdr:ext cx="2318135" cy="436786"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="65" name="ZoneTexte 64"/>
@@ -2912,8 +2910,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9801226" y="1933575"/>
-          <a:ext cx="1755031" cy="436786"/>
+          <a:off x="9523039" y="1933575"/>
+          <a:ext cx="2318135" cy="436786"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2943,7 +2941,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>v(fn, MC) &amp;&amp; v(fn, M'C) &amp;&amp;</a:t>
+            <a:t>v(fn, GW, MC) &amp;&amp; v(fn, GW, M'C) &amp;&amp;</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2959,12 +2957,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>225983</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>706433</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3550972" cy="436786"/>
+    <xdr:ext cx="4114075" cy="436786"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="68" name="ZoneTexte 67"/>
@@ -2972,8 +2970,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5550458" y="3343275"/>
-          <a:ext cx="3550972" cy="436786"/>
+          <a:off x="5278433" y="3343275"/>
+          <a:ext cx="4114075" cy="436786"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3003,7 +3001,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>(v(fn, MC) &amp;&amp; v(fn, M'C) &amp;&amp; longueur chemin plus long) ||</a:t>
+            <a:t>(v(fn, GW, MC) &amp;&amp; v(fn, GW, M'C) &amp;&amp; longueur chemin plus long) ||</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3022,7 +3020,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>v(fn, MC) &amp;&amp; v(fn, M'C))</a:t>
+            <a:t>v(fn, GW, MC) &amp;&amp; v(fn, GW, M'C))</a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
@@ -3032,12 +3030,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>232962</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>955038</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="984307" cy="436786"/>
+    <xdr:ext cx="1265859" cy="436786"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="69" name="ZoneTexte 68"/>
@@ -3045,8 +3043,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8795937" y="2867025"/>
-          <a:ext cx="984307" cy="436786"/>
+          <a:off x="8507803" y="2867025"/>
+          <a:ext cx="1265859" cy="436786"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3076,14 +3074,14 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>!v(fn, MC) &amp;&amp;</a:t>
+            <a:t>!v(fn, GW, MC) &amp;&amp;</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>!v(fn, M'C)</a:t>
+            <a:t>!v(fn, GW, M'C)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3184,11 +3182,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>564098</xdr:colOff>
+      <xdr:colOff>531589</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>37712</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="970907" cy="444289"/>
+    <xdr:ext cx="1035926" cy="444289"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="71" name="ZoneTexte 70"/>
@@ -3196,8 +3194,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8117423" y="1561712"/>
-          <a:ext cx="970907" cy="444289"/>
+          <a:off x="8084354" y="1561712"/>
+          <a:ext cx="1035926" cy="444289"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3291,7 +3289,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>!v(fn, MC) </a:t>
+            <a:t>!v(fn, GA, MA) </a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
@@ -3488,7 +3486,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>CAS 1 : Traitement de chaque action de la trace</a:t>
+            <a:t>CAS 0 : Traitement de chaque action de la trace</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3663,7 +3661,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>CAS "Fin" : gestion des actions manquantes en</a:t>
+            <a:t>CAS 6 "Fin" : gestion des actions manquantes en</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
@@ -3843,7 +3841,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>CAS 1.2 : Cas des actions acceptées par le jeu</a:t>
+            <a:t>CAS 1 : Cas des actions acceptées par le jeu</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4062,7 +4060,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>CAS "Dans espace filtré"</a:t>
+            <a:t>CAS 2 "Dans espace filtré"</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4245,7 +4243,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>CAS "Vers solution"</a:t>
+            <a:t>CAS 2_1 "Vers solution"</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4421,7 +4419,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>CAS "Stagnation"</a:t>
+            <a:t>CAS 2_2 "Stagnation"</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4611,7 +4609,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>CAS "</a:t>
+            <a:t>CAS 3 "</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
@@ -4837,7 +4835,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>CAS "Hors espace filtré depuis MiC"</a:t>
+            <a:t>CAS 4 "Hors espace filtré depuis MiC"</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5020,7 +5018,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>CAS "Puits"</a:t>
+            <a:t>CAS 5 "Tendance"</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5077,7 +5075,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>CAS 1.1 : Cas des actions refusées par le jeu</a:t>
+            <a:t>Cas des actions refusées par le jeu</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5659,10 +5657,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A32:L132"/>
+  <dimension ref="A32:L129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K126" sqref="K126"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5697,7 +5695,7 @@
         <v>89</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -5705,7 +5703,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -5738,9 +5736,15 @@
       <c r="B38" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="12"/>
+      <c r="C38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="9"/>
@@ -5769,7 +5773,7 @@
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
       <c r="J39" s="5" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="K39" s="7"/>
     </row>
@@ -5798,70 +5802,106 @@
       <c r="A41" s="3">
         <v>1</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="B41" s="3">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3">
+        <v>1</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="8"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="K41" s="3"/>
+      <c r="I41" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="J41" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
+      <c r="A42" s="3">
+        <v>1</v>
+      </c>
+      <c r="B42" s="3">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3">
+        <v>1</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0</v>
+      </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="20"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="K42" s="3"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
+      <c r="A43" s="3">
+        <v>1</v>
+      </c>
+      <c r="B43" s="3">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="20"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="K43" s="3"/>
     </row>
-    <row r="44" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J44" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K44" s="6" t="s">
-        <v>17</v>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>1</v>
+      </c>
+      <c r="B44" s="3">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3">
+        <v>1</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0</v>
+      </c>
+      <c r="E44" s="3">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -5869,25 +5909,21 @@
         <v>1</v>
       </c>
       <c r="B45" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="8"/>
-      <c r="I45" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="J45" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="I45" s="35"/>
+      <c r="J45" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="K45" s="3"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
@@ -5896,159 +5932,156 @@
       <c r="B46" s="3">
         <v>1</v>
       </c>
-      <c r="C46" s="3">
-        <v>0</v>
-      </c>
+      <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="35"/>
-      <c r="J46" s="19" t="s">
-        <v>28</v>
+      <c r="H46" s="8"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="37" t="s">
+        <v>140</v>
       </c>
       <c r="K46" s="3"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <v>1</v>
-      </c>
-      <c r="B47" s="3">
-        <v>0</v>
-      </c>
-      <c r="C47" s="3">
-        <v>1</v>
-      </c>
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="8"/>
-      <c r="I47" s="35"/>
-      <c r="J47" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="I47" s="1"/>
+      <c r="J47" s="31"/>
       <c r="K47" s="3"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
-        <v>1</v>
-      </c>
-      <c r="B48" s="3">
-        <v>0</v>
-      </c>
-      <c r="C48" s="3">
-        <v>0</v>
-      </c>
+      <c r="A48" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="35"/>
-      <c r="J48" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
-        <v>0</v>
-      </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="35"/>
-      <c r="J49" s="20" t="s">
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="12"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J49" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K49" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="25">
+        <v>1</v>
+      </c>
+      <c r="B50" s="24"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="J50" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" s="11">
+        <v>1</v>
+      </c>
+      <c r="J51" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>0</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" s="11">
+        <v>0</v>
+      </c>
+      <c r="H52" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" t="s">
+        <v>20</v>
+      </c>
+      <c r="J52" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="K49" s="3"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="31"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="3"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-    </row>
-    <row r="52" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B52" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E52" s="12"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J52" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K52" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="25">
+      <c r="K52" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>0</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53" s="11">
         <v>1</v>
       </c>
-      <c r="B53" s="24"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="26"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="I53" s="28" t="s">
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
         <v>20</v>
       </c>
-      <c r="J53" s="14" t="s">
-        <v>63</v>
+      <c r="J53" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="K53" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -6056,13 +6089,22 @@
         <v>0</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54" s="11">
         <v>1</v>
       </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="H54" t="s">
+        <v>20</v>
+      </c>
       <c r="J54" s="18" t="s">
-        <v>129</v>
+        <v>144</v>
+      </c>
+      <c r="K54" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -6070,167 +6112,149 @@
         <v>0</v>
       </c>
       <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55" s="11">
+        <v>0</v>
+      </c>
+      <c r="J55" s="18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" s="11"/>
+      <c r="J56" s="18"/>
+    </row>
+    <row r="57" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" s="11"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="J57" s="18"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="22">
         <v>1</v>
       </c>
-      <c r="C55" s="11">
-        <v>0</v>
-      </c>
-      <c r="H55" t="s">
-        <v>18</v>
-      </c>
-      <c r="I55" t="s">
+      <c r="B58" s="11"/>
+      <c r="I58" t="s">
         <v>20</v>
       </c>
-      <c r="J55" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="K55" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>0</v>
-      </c>
-      <c r="B56">
-        <v>0</v>
-      </c>
-      <c r="C56" s="11">
+      <c r="J58" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="22">
+        <v>0</v>
+      </c>
+      <c r="B59" s="11"/>
+      <c r="I59" t="s">
+        <v>20</v>
+      </c>
+      <c r="J59" s="18"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="22"/>
+      <c r="B60" s="11"/>
+      <c r="J60" s="18"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A64" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K64" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65">
         <v>1</v>
       </c>
-      <c r="D56">
+      <c r="B65">
         <v>1</v>
       </c>
-      <c r="H56" t="s">
-        <v>20</v>
-      </c>
-      <c r="J56" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="K56" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>0</v>
-      </c>
-      <c r="B57">
-        <v>0</v>
-      </c>
-      <c r="C57" s="11">
+      <c r="C65">
         <v>1</v>
       </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="H57" t="s">
-        <v>20</v>
-      </c>
-      <c r="J57" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="K57" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>0</v>
-      </c>
-      <c r="B58">
-        <v>0</v>
-      </c>
-      <c r="C58" s="11">
-        <v>0</v>
-      </c>
-      <c r="J58" s="18" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B59" s="11"/>
-      <c r="J59" s="18"/>
-    </row>
-    <row r="60" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B60" s="11"/>
-      <c r="H60" s="21"/>
-      <c r="I60" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="J60" s="18"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="22">
+      <c r="J65" s="18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66">
         <v>1</v>
       </c>
-      <c r="B61" s="11"/>
-      <c r="I61" t="s">
-        <v>20</v>
-      </c>
-      <c r="J61" s="18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="22">
-        <v>0</v>
-      </c>
-      <c r="B62" s="11"/>
-      <c r="I62" t="s">
-        <v>20</v>
-      </c>
-      <c r="J62" s="18"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
-      <c r="B63" s="11"/>
-      <c r="J63" s="18"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="30" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A67" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B67" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D67" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E67" s="10"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="10"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K67" s="13" t="s">
-        <v>17</v>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="J66" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="J67" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="K67" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -6238,295 +6262,289 @@
         <v>1</v>
       </c>
       <c r="B68">
-        <v>1</v>
-      </c>
-      <c r="C68">
-        <v>1</v>
-      </c>
-      <c r="J68" s="18" t="s">
-        <v>133</v>
+        <v>0</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K68" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B69">
         <v>1</v>
       </c>
-      <c r="C69">
-        <v>0</v>
-      </c>
-      <c r="D69">
-        <v>1</v>
-      </c>
       <c r="J69" s="18" t="s">
-        <v>134</v>
+        <v>150</v>
+      </c>
+      <c r="K69" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B70">
-        <v>1</v>
-      </c>
-      <c r="C70">
-        <v>0</v>
-      </c>
-      <c r="D70">
         <v>0</v>
       </c>
       <c r="J70" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="K70" t="s">
-        <v>61</v>
+        <v>151</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>1</v>
-      </c>
-      <c r="B71">
-        <v>0</v>
-      </c>
-      <c r="J71" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K71" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>0</v>
-      </c>
-      <c r="B72">
-        <v>1</v>
-      </c>
-      <c r="J72" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="K72" t="s">
-        <v>62</v>
-      </c>
+      <c r="A71" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J71" s="18"/>
+    </row>
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H72" s="4"/>
+      <c r="J72" s="18"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>0</v>
-      </c>
-      <c r="B73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J73" s="18" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J74" s="18"/>
-    </row>
-    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="H75" s="4"/>
-      <c r="J75" s="18"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76">
+      <c r="A74">
+        <v>0</v>
+      </c>
+      <c r="B74">
         <v>1</v>
       </c>
-      <c r="J76" s="18" t="s">
-        <v>116</v>
+      <c r="J74" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>0</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="J75" s="18" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>0</v>
-      </c>
-      <c r="B77">
+      <c r="B77" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B78" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D78" s="12"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K78" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B79">
         <v>1</v>
       </c>
-      <c r="J77" s="18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>0</v>
-      </c>
-      <c r="B78">
-        <v>0</v>
-      </c>
-      <c r="J78" s="18" t="s">
-        <v>119</v>
+      <c r="J79" t="s">
+        <v>41</v>
+      </c>
+      <c r="K79" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B80" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B81" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C81" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D81" s="12"/>
-      <c r="H81" s="4"/>
-      <c r="I81" s="4"/>
-      <c r="J81" s="13" t="s">
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="J80" t="s">
+        <v>31</v>
+      </c>
+      <c r="K80" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="J81" t="s">
+        <v>42</v>
+      </c>
+      <c r="K81" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B83" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="B84" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K81" s="13" t="s">
+      <c r="K84" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B82">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B85">
         <v>1</v>
       </c>
-      <c r="J82" t="s">
-        <v>41</v>
-      </c>
-      <c r="K82" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B83">
-        <v>0</v>
-      </c>
-      <c r="C83">
+      <c r="J85" t="s">
+        <v>40</v>
+      </c>
+      <c r="K85" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
         <v>1</v>
       </c>
-      <c r="J83" t="s">
-        <v>31</v>
-      </c>
-      <c r="K83" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B84">
-        <v>0</v>
-      </c>
-      <c r="C84">
-        <v>0</v>
-      </c>
-      <c r="J84" t="s">
+      <c r="J86" t="s">
+        <v>40</v>
+      </c>
+      <c r="K86" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="J87" t="s">
+        <v>59</v>
+      </c>
+      <c r="K87" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" s="30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C92" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4"/>
+      <c r="J92" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K92" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>1</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="J93" t="s">
+        <v>19</v>
+      </c>
+      <c r="K93" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>1</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="J94" t="s">
+        <v>45</v>
+      </c>
+      <c r="K94" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>0</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="J95" t="s">
         <v>42</v>
       </c>
-      <c r="K84" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B86" s="8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="B87" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="C87" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="H87" s="4"/>
-      <c r="I87" s="4"/>
-      <c r="J87" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K87" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B88">
-        <v>1</v>
-      </c>
-      <c r="J88" t="s">
-        <v>40</v>
-      </c>
-      <c r="K88" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B89">
-        <v>0</v>
-      </c>
-      <c r="C89">
-        <v>1</v>
-      </c>
-      <c r="J89" t="s">
-        <v>40</v>
-      </c>
-      <c r="K89" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B90">
-        <v>0</v>
-      </c>
-      <c r="C90">
-        <v>0</v>
-      </c>
-      <c r="J90" t="s">
-        <v>59</v>
-      </c>
-      <c r="K90" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="30" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B95" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="C95" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="H95" s="4"/>
-      <c r="I95" s="4"/>
-      <c r="J95" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K95" s="13" t="s">
-        <v>17</v>
+      <c r="K95" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -6535,291 +6553,316 @@
         <v>19</v>
       </c>
       <c r="K96" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97">
+        <v>0</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="J97" t="s">
+        <v>59</v>
+      </c>
+      <c r="K97" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" s="23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A101" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B101" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I101" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J101" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K101" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L101" s="7"/>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A102" s="25">
         <v>1</v>
       </c>
-      <c r="C97">
-        <v>0</v>
-      </c>
-      <c r="J97" t="s">
-        <v>45</v>
-      </c>
-      <c r="K97" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>0</v>
-      </c>
-      <c r="B98">
+      <c r="B102" s="25"/>
+      <c r="C102" s="25"/>
+      <c r="D102" s="25"/>
+      <c r="E102" s="25"/>
+      <c r="F102" s="26"/>
+      <c r="G102" s="26"/>
+      <c r="H102" s="28"/>
+      <c r="I102" s="28"/>
+      <c r="J102" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="L102" s="3"/>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A103" s="11">
+        <v>0</v>
+      </c>
+      <c r="B103">
         <v>1</v>
       </c>
-      <c r="J98" t="s">
-        <v>42</v>
-      </c>
-      <c r="K98" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>0</v>
-      </c>
-      <c r="B99">
-        <v>0</v>
-      </c>
-      <c r="C99">
+      <c r="H103" t="s">
+        <v>18</v>
+      </c>
+      <c r="I103" t="s">
+        <v>20</v>
+      </c>
+      <c r="J103" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="K103" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104" s="11">
+        <v>0</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="H104" t="s">
+        <v>18</v>
+      </c>
+      <c r="I104" t="s">
+        <v>20</v>
+      </c>
+      <c r="J104" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="K104" s="3"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A106" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A107" s="30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="H109" s="4"/>
+      <c r="I109" s="4"/>
+      <c r="J109" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K109" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A110">
         <v>1</v>
       </c>
-      <c r="J99" t="s">
-        <v>19</v>
-      </c>
-      <c r="K99" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>0</v>
-      </c>
-      <c r="B100">
-        <v>0</v>
-      </c>
-      <c r="C100">
-        <v>0</v>
-      </c>
-      <c r="J100" t="s">
-        <v>59</v>
-      </c>
-      <c r="K100" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A102" s="8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A103" s="23" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A104" s="12" t="s">
+      <c r="J110" t="s">
+        <v>80</v>
+      </c>
+      <c r="K110" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>0</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="J111" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="K111" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>0</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+      <c r="J112" t="s">
+        <v>81</v>
+      </c>
+      <c r="K112" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B114" s="8"/>
+      <c r="C114" s="8"/>
+      <c r="D114" s="8"/>
+      <c r="E114" s="8"/>
+      <c r="F114" s="8"/>
+      <c r="G114" s="8"/>
+      <c r="H114" s="8"/>
+      <c r="I114" s="8"/>
+      <c r="J114" s="8"/>
+      <c r="K114" s="8"/>
+    </row>
+    <row r="115" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A115" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B115" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C115" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D115" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="B104" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C104" s="4"/>
-      <c r="D104" s="4"/>
-      <c r="E104" s="4"/>
-      <c r="F104" s="4"/>
-      <c r="G104" s="4"/>
-      <c r="H104" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I104" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J104" s="13" t="s">
+      <c r="E115" s="13"/>
+      <c r="F115" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G115" s="13"/>
+      <c r="H115" s="13"/>
+      <c r="I115" s="13"/>
+      <c r="J115" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K104" s="13" t="s">
+      <c r="K115" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="L104" s="7"/>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A105" s="25">
+    </row>
+    <row r="116" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="14">
         <v>1</v>
       </c>
-      <c r="B105" s="25"/>
-      <c r="C105" s="25"/>
-      <c r="D105" s="25"/>
-      <c r="E105" s="25"/>
-      <c r="F105" s="26"/>
-      <c r="G105" s="26"/>
-      <c r="H105" s="28"/>
-      <c r="I105" s="28"/>
-      <c r="J105" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="L105" s="3"/>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A106" s="11">
-        <v>0</v>
-      </c>
-      <c r="B106">
+      <c r="C116" s="14"/>
+      <c r="E116" s="14"/>
+      <c r="F116" s="14"/>
+      <c r="G116" s="14"/>
+      <c r="H116" s="14"/>
+      <c r="I116" s="14"/>
+      <c r="J116" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K116" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117" s="14">
+        <v>0</v>
+      </c>
+      <c r="B117">
         <v>1</v>
       </c>
-      <c r="H106" t="s">
-        <v>18</v>
-      </c>
-      <c r="I106" t="s">
-        <v>20</v>
-      </c>
-      <c r="J106" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="K106" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A107" s="11">
-        <v>0</v>
-      </c>
-      <c r="B107">
-        <v>0</v>
-      </c>
-      <c r="H107" t="s">
-        <v>18</v>
-      </c>
-      <c r="I107" t="s">
-        <v>20</v>
-      </c>
-      <c r="J107" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="K107" s="3"/>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A109" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A110" s="30" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A111" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A112" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B112" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C112" s="4"/>
-      <c r="D112" s="4"/>
-      <c r="H112" s="4"/>
-      <c r="I112" s="4"/>
-      <c r="J112" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K112" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A113">
+      <c r="C117" s="14"/>
+      <c r="E117" s="14"/>
+      <c r="F117" s="14"/>
+      <c r="G117" s="14"/>
+      <c r="H117" s="14"/>
+      <c r="I117" s="14"/>
+      <c r="J117" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="K117" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118" s="14">
+        <v>0</v>
+      </c>
+      <c r="B118">
+        <v>0</v>
+      </c>
+      <c r="C118" s="14">
         <v>1</v>
       </c>
-      <c r="J113" t="s">
-        <v>80</v>
-      </c>
-      <c r="K113" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A114">
-        <v>0</v>
-      </c>
-      <c r="B114">
+      <c r="E118" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="F118" s="14">
         <v>1</v>
       </c>
-      <c r="J114" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="K114" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A115">
-        <v>0</v>
-      </c>
-      <c r="B115">
-        <v>0</v>
-      </c>
-      <c r="J115" t="s">
-        <v>81</v>
-      </c>
-      <c r="K115" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A117" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B117" s="8"/>
-      <c r="C117" s="8"/>
-      <c r="D117" s="8"/>
-      <c r="E117" s="8"/>
-      <c r="F117" s="8"/>
-      <c r="G117" s="8"/>
-      <c r="H117" s="8"/>
-      <c r="I117" s="8"/>
-      <c r="J117" s="8"/>
-      <c r="K117" s="8"/>
-    </row>
-    <row r="118" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A118" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="B118" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C118" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D118" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="E118" s="13"/>
-      <c r="F118" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G118" s="13"/>
-      <c r="H118" s="13"/>
-      <c r="I118" s="13"/>
-      <c r="J118" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K118" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G118" s="14"/>
+      <c r="H118" s="14"/>
+      <c r="I118" s="14"/>
+      <c r="J118" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="K118" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="14">
+        <v>0</v>
+      </c>
+      <c r="B119">
+        <v>0</v>
+      </c>
+      <c r="C119" s="14">
         <v>1</v>
       </c>
-      <c r="C119" s="14"/>
-      <c r="E119" s="14"/>
-      <c r="F119" s="14"/>
+      <c r="E119" s="36"/>
+      <c r="F119" s="14">
+        <v>0</v>
+      </c>
       <c r="G119" s="14"/>
       <c r="H119" s="14"/>
       <c r="I119" s="14"/>
-      <c r="J119" s="14" t="s">
-        <v>35</v>
+      <c r="J119" s="15" t="s">
+        <v>128</v>
       </c>
       <c r="K119" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
@@ -6827,19 +6870,28 @@
         <v>0</v>
       </c>
       <c r="B120">
+        <v>0</v>
+      </c>
+      <c r="C120" s="14">
+        <v>0</v>
+      </c>
+      <c r="D120" s="14">
         <v>1</v>
       </c>
-      <c r="C120" s="14"/>
-      <c r="E120" s="14"/>
-      <c r="F120" s="14"/>
+      <c r="E120" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="F120" s="14">
+        <v>1</v>
+      </c>
       <c r="G120" s="14"/>
       <c r="H120" s="14"/>
       <c r="I120" s="14"/>
       <c r="J120" s="15" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="K120" s="14" t="s">
-        <v>151</v>
+        <v>37</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
@@ -6850,22 +6902,23 @@
         <v>0</v>
       </c>
       <c r="C121" s="14">
+        <v>0</v>
+      </c>
+      <c r="D121" s="14">
         <v>1</v>
       </c>
-      <c r="E121" s="36" t="s">
-        <v>147</v>
-      </c>
+      <c r="E121" s="36"/>
       <c r="F121" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G121" s="14"/>
       <c r="H121" s="14"/>
-      <c r="I121" s="14"/>
+      <c r="I121" s="32"/>
       <c r="J121" s="15" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="K121" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
@@ -6875,121 +6928,41 @@
       <c r="B122">
         <v>0</v>
       </c>
-      <c r="C122" s="14">
-        <v>1</v>
-      </c>
-      <c r="E122" s="36"/>
-      <c r="F122" s="14">
-        <v>0</v>
-      </c>
-      <c r="G122" s="14"/>
-      <c r="H122" s="14"/>
-      <c r="I122" s="14"/>
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
       <c r="J122" s="15" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="K122" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A123" s="14">
-        <v>0</v>
-      </c>
-      <c r="B123">
-        <v>0</v>
-      </c>
-      <c r="C123" s="14">
-        <v>0</v>
-      </c>
-      <c r="D123" s="14">
-        <v>1</v>
-      </c>
-      <c r="E123" s="36" t="s">
-        <v>148</v>
-      </c>
-      <c r="F123" s="14">
-        <v>1</v>
-      </c>
-      <c r="G123" s="14"/>
-      <c r="H123" s="14"/>
-      <c r="I123" s="14"/>
-      <c r="J123" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="K123" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A124" s="14">
-        <v>0</v>
-      </c>
-      <c r="B124">
-        <v>0</v>
-      </c>
-      <c r="C124" s="14">
-        <v>0</v>
-      </c>
-      <c r="D124" s="14">
-        <v>1</v>
-      </c>
-      <c r="E124" s="36"/>
-      <c r="F124" s="14">
-        <v>0</v>
-      </c>
-      <c r="G124" s="14"/>
-      <c r="H124" s="14"/>
-      <c r="I124" s="33"/>
-      <c r="J124" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="K124" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A125" s="14">
-        <v>0</v>
-      </c>
-      <c r="B125">
-        <v>0</v>
-      </c>
-      <c r="C125">
-        <v>0</v>
-      </c>
-      <c r="D125">
-        <v>0</v>
-      </c>
-      <c r="J125" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="K125" s="14" t="s">
-        <v>152</v>
-      </c>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J126" s="15"/>
+      <c r="K126" s="14"/>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J127" s="15"/>
+      <c r="K127" s="14"/>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J128" s="15"/>
+      <c r="K128" s="14"/>
     </row>
     <row r="129" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J129" s="15"/>
       <c r="K129" s="14"/>
     </row>
-    <row r="130" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J130" s="15"/>
-      <c r="K130" s="14"/>
-    </row>
-    <row r="131" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J131" s="15"/>
-      <c r="K131" s="14"/>
-    </row>
-    <row r="132" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J132" s="15"/>
-      <c r="K132" s="14"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A32:K32"/>
-    <mergeCell ref="I45:I49"/>
-    <mergeCell ref="E121:E122"/>
-    <mergeCell ref="E123:E124"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="E120:E121"/>
+    <mergeCell ref="I41:I45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajout de la version 10 de l'algo de labellisation Intégration de paramètres pour une utilisation en ligne de commande avec commmunication possible par socket
</commit_message>
<xml_diff>
--- a/docs/MatriceLabellisationV9.2.xlsx
+++ b/docs/MatriceLabellisationV9.2.xlsx
@@ -5485,7 +5485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -5659,8 +5659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A32:L129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>